<commit_message>
issues fixes and scenarios implementation
</commit_message>
<xml_diff>
--- a/public/samples/purchase.xlsx
+++ b/public/samples/purchase.xlsx
@@ -13,6 +13,44 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Tax Period</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>Invoice Number</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Item subject to taxes</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Goods Description</t>
+  </si>
+  <si>
+    <t>Non Taxable Purchases</t>
+  </si>
+  <si>
+    <t>Local Purchase (Taxable Value)</t>
+  </si>
+  <si>
+    <t>Imports (Taxable Value)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +84,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,12 +386,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="60">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>